<commit_message>
Modified Brilliance with prorportions
</commit_message>
<xml_diff>
--- a/Diamond_Proportions.xlsx
+++ b/Diamond_Proportions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DiamondRayTracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAA9D28-049F-4A66-BE71-C600A258C017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4DC963-B912-496F-B2D9-9758ABAB7BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1ECD17EE-4C70-4896-8AF6-708326DFBDFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>Proportion 1</t>
   </si>
@@ -58,6 +59,42 @@
   </si>
   <si>
     <t>Proportion 3</t>
+  </si>
+  <si>
+    <t>Crown Facets Split</t>
+  </si>
+  <si>
+    <t>50:50</t>
+  </si>
+  <si>
+    <t>Pavillion Facets split</t>
+  </si>
+  <si>
+    <t>80:20</t>
+  </si>
+  <si>
+    <t>Crown Angle</t>
+  </si>
+  <si>
+    <t>Pavillion Angle</t>
+  </si>
+  <si>
+    <t>Crown Split</t>
+  </si>
+  <si>
+    <t>Pavillion Split</t>
+  </si>
+  <si>
+    <t>Proportion 4</t>
+  </si>
+  <si>
+    <t>Proportion 5</t>
+  </si>
+  <si>
+    <t>Proportion 6</t>
+  </si>
+  <si>
+    <t>Proportion 7</t>
   </si>
 </sst>
 </file>
@@ -95,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -118,11 +155,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -136,6 +210,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -158,15 +244,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -196,7 +282,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7117080" y="2446020"/>
+          <a:off x="7528560" y="2590800"/>
           <a:ext cx="4572000" cy="3429000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -219,15 +305,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1897</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>131437</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -250,7 +336,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="358140" y="1524000"/>
+          <a:off x="480060" y="3665220"/>
           <a:ext cx="5654040" cy="2501257"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -262,16 +348,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>708661</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>175261</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38070</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>502921</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>45690</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -294,7 +380,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6690361" y="45720"/>
+          <a:off x="708661" y="6271260"/>
           <a:ext cx="5356860" cy="2369790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -604,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28F9BF8-5CF6-4888-B086-4549489BDDE6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,45 +705,93 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -666,15 +800,31 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1">
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1">
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,20 +837,48 @@
       </c>
       <c r="D4" s="4">
         <f>$D$3*E4/100</f>
-        <v>1.1340000000000001</v>
+        <v>2.16</v>
       </c>
       <c r="E4" s="1">
         <v>54</v>
       </c>
       <c r="F4" s="4">
         <f>$F$3*G4/100</f>
-        <v>1.3020000000000003</v>
+        <v>2.48</v>
       </c>
       <c r="G4" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="4">
+        <f>$F$3*I4/100</f>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="I4" s="1">
+        <v>57</v>
+      </c>
+      <c r="J4" s="4">
+        <f>$F$3*K4/100</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="K4" s="1">
+        <v>56</v>
+      </c>
+      <c r="L4" s="4">
+        <f>$F$3*M4/100</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="M4" s="1">
+        <v>56</v>
+      </c>
+      <c r="N4" s="4">
+        <f>$F$3*O4/100</f>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="O4" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -713,20 +891,48 @@
       </c>
       <c r="D5" s="4">
         <f t="shared" ref="D5:D8" si="0">$D$3*E5/100</f>
-        <v>8.4000000000000005E-2</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
       </c>
       <c r="F5" s="4">
         <f>$F$3*G5/100</f>
-        <v>9.4500000000000015E-2</v>
+        <v>0.18</v>
       </c>
       <c r="G5" s="1">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="4">
+        <f>$F$3*I5/100</f>
+        <v>0.16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+      <c r="J5" s="4">
+        <f>$F$3*K5/100</f>
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4">
+        <f>$F$3*M5/100</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M5" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="N5" s="4">
+        <f>$F$3*O5/100</f>
+        <v>0.2</v>
+      </c>
+      <c r="O5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -739,20 +945,48 @@
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>0.88200000000000001</v>
+        <v>1.68</v>
       </c>
       <c r="E6" s="1">
         <v>42</v>
       </c>
       <c r="F6" s="4">
         <f>$F$3*G6/100</f>
-        <v>0.95550000000000002</v>
+        <v>1.82</v>
       </c>
       <c r="G6" s="1">
         <v>45.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="4">
+        <f>$F$3*I6/100</f>
+        <v>1.78</v>
+      </c>
+      <c r="I6" s="1">
+        <v>44.5</v>
+      </c>
+      <c r="J6" s="4">
+        <f>$F$3*K6/100</f>
+        <v>1.72</v>
+      </c>
+      <c r="K6" s="1">
+        <v>43</v>
+      </c>
+      <c r="L6" s="4">
+        <f>$F$3*M6/100</f>
+        <v>1.72</v>
+      </c>
+      <c r="M6" s="1">
+        <v>43</v>
+      </c>
+      <c r="N6" s="4">
+        <f>$F$3*O6/100</f>
+        <v>1.72</v>
+      </c>
+      <c r="O6" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -765,20 +999,48 @@
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>0.29400000000000004</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E7" s="1">
         <v>14</v>
       </c>
       <c r="F7" s="4">
         <f>$F$3*G7/100</f>
-        <v>0.29400000000000004</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G7" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="4">
+        <f>$F$3*I7/100</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I7" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="J7" s="4">
+        <f>$F$3*K7/100</f>
+        <v>0.62</v>
+      </c>
+      <c r="K7" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="L7" s="4">
+        <f>$F$3*M7/100</f>
+        <v>0.66</v>
+      </c>
+      <c r="M7" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="N7" s="4">
+        <f>$F$3*O7/100</f>
+        <v>0.64</v>
+      </c>
+      <c r="O7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -791,26 +1053,293 @@
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>1.26</v>
+        <v>2.4</v>
       </c>
       <c r="E8" s="1">
         <v>60</v>
       </c>
       <c r="F8" s="4">
         <f>$F$3*G8/100</f>
-        <v>1.3545000000000003</v>
+        <v>2.58</v>
       </c>
       <c r="G8" s="1">
         <v>64.5</v>
       </c>
+      <c r="H8" s="4">
+        <f>$F$3*I8/100</f>
+        <v>2.508</v>
+      </c>
+      <c r="I8" s="1">
+        <v>62.7</v>
+      </c>
+      <c r="J8" s="4">
+        <f>$F$3*K8/100</f>
+        <v>2.524</v>
+      </c>
+      <c r="K8" s="1">
+        <v>63.1</v>
+      </c>
+      <c r="L8" s="4">
+        <f>$F$3*M8/100</f>
+        <v>2.512</v>
+      </c>
+      <c r="M8" s="1">
+        <v>62.8</v>
+      </c>
+      <c r="N8" s="4">
+        <f>$F$3*O8/100</f>
+        <v>2.5680000000000001</v>
+      </c>
+      <c r="O8" s="1">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>30.9</v>
+      </c>
+      <c r="F9">
+        <v>35.9</v>
+      </c>
+      <c r="H9">
+        <v>34</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9">
+        <v>35</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9">
+        <v>36.5</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9">
+        <v>37</v>
+      </c>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>42.4</v>
+      </c>
+      <c r="H10">
+        <v>41.6</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10">
+        <v>40.6</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2878877B-1B04-497B-9A2A-1B776049E7C3}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.41</v>
+      </c>
+      <c r="C4" s="3">
+        <f>B4/$B$3*100</f>
+        <v>54.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="3">
+        <f>B5/$B$3*100</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="C6" s="3">
+        <f>B6/$B$3*100</f>
+        <v>44.400000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="C7" s="3">
+        <f>B7/$B$3*100</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.13</v>
+      </c>
+      <c r="C8" s="3">
+        <f>B8/$B$3*100</f>
+        <v>61.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <f>0.8*$B3/2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f>0.2*$B3/2</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>